<commit_message>
Timesheet_entries from 14/8/2012 to 20/8/2012
</commit_message>
<xml_diff>
--- a/Time_sheet.xlsx
+++ b/Time_sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="17">
   <si>
     <t>Date</t>
   </si>
@@ -420,8 +420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:E542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1116,41 +1116,83 @@
         <f t="shared" si="0"/>
         <v>41135</v>
       </c>
+      <c r="D62" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="2:5">
       <c r="C63" s="2">
         <f t="shared" si="0"/>
         <v>41136</v>
       </c>
+      <c r="D63" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="2:5">
       <c r="C64" s="2">
         <f t="shared" si="0"/>
         <v>41137</v>
       </c>
+      <c r="D64" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="3:5">
       <c r="C65" s="2">
         <f t="shared" si="0"/>
         <v>41138</v>
       </c>
+      <c r="D65" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65">
+        <v>1</v>
+      </c>
     </row>
     <row r="66" spans="3:5">
       <c r="C66" s="2">
         <f t="shared" si="0"/>
         <v>41139</v>
       </c>
+      <c r="D66" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="3:5">
       <c r="C67" s="2">
         <f t="shared" si="0"/>
         <v>41140</v>
       </c>
+      <c r="D67" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
     </row>
     <row r="68" spans="3:5">
       <c r="C68" s="2">
         <f t="shared" si="0"/>
         <v>41141</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="3:5">
@@ -1193,7 +1235,7 @@
       </c>
       <c r="E75">
         <f>SUM(E5:E74)</f>
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="76" spans="3:5">

</xml_diff>

<commit_message>
Timesheet_entries from 21/8/2012 to 31/8/2012
</commit_message>
<xml_diff>
--- a/Time_sheet.xlsx
+++ b/Time_sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Tiers in a Bank data warehouse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Report for  2nd deliverable </t>
   </si>
 </sst>
 </file>
@@ -420,14 +423,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:E542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="E121" sqref="E121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="4" max="4" width="48.140625" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" customWidth="1"/>
     <col min="5" max="5" width="21" customWidth="1"/>
   </cols>
   <sheetData>
@@ -804,7 +807,7 @@
     </row>
     <row r="37" spans="3:5">
       <c r="C37" s="2">
-        <f t="shared" ref="C37:C73" si="0">C36+1</f>
+        <f t="shared" ref="C37:C88" si="0">C36+1</f>
         <v>41110</v>
       </c>
       <c r="D37" t="s">
@@ -1200,88 +1203,186 @@
         <f t="shared" si="0"/>
         <v>41142</v>
       </c>
+      <c r="D69" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" spans="3:5">
       <c r="C70" s="2">
         <f t="shared" si="0"/>
         <v>41143</v>
       </c>
+      <c r="D70" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
     </row>
     <row r="71" spans="3:5">
       <c r="C71" s="2">
         <f t="shared" si="0"/>
         <v>41144</v>
       </c>
+      <c r="D71" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="3:5">
       <c r="C72" s="2">
         <f t="shared" si="0"/>
         <v>41145</v>
       </c>
+      <c r="D72" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
     </row>
     <row r="73" spans="3:5">
       <c r="C73" s="2">
         <f t="shared" si="0"/>
         <v>41146</v>
       </c>
+      <c r="D73" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
     </row>
     <row r="74" spans="3:5">
-      <c r="C74" s="2"/>
+      <c r="C74" s="2">
+        <f t="shared" si="0"/>
+        <v>41147</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74">
+        <v>2</v>
+      </c>
     </row>
     <row r="75" spans="3:5">
-      <c r="C75" s="2"/>
-      <c r="D75" t="s">
-        <v>11</v>
+      <c r="C75" s="2">
+        <f t="shared" si="0"/>
+        <v>41148</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="E75">
-        <f>SUM(E5:E74)</f>
-        <v>77</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="3:5">
-      <c r="C76" s="2"/>
+      <c r="C76" s="2">
+        <f t="shared" si="0"/>
+        <v>41149</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
     </row>
     <row r="77" spans="3:5">
-      <c r="C77" s="2"/>
+      <c r="C77" s="2">
+        <f t="shared" si="0"/>
+        <v>41150</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E77">
+        <v>1</v>
+      </c>
     </row>
     <row r="78" spans="3:5">
-      <c r="C78" s="2"/>
-      <c r="D78" t="s">
-        <v>12</v>
+      <c r="C78" s="2">
+        <f t="shared" si="0"/>
+        <v>41151</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="E78">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="3:5">
-      <c r="C79" s="2"/>
+      <c r="C79" s="2">
+        <f t="shared" si="0"/>
+        <v>41152</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E79">
+        <v>2</v>
+      </c>
     </row>
     <row r="80" spans="3:5">
-      <c r="C80" s="2"/>
+      <c r="C80" s="2">
+        <f t="shared" si="0"/>
+        <v>41153</v>
+      </c>
     </row>
     <row r="81" spans="3:3">
-      <c r="C81" s="2"/>
+      <c r="C81" s="2">
+        <f t="shared" si="0"/>
+        <v>41154</v>
+      </c>
     </row>
     <row r="82" spans="3:3">
-      <c r="C82" s="2"/>
+      <c r="C82" s="2">
+        <f t="shared" si="0"/>
+        <v>41155</v>
+      </c>
     </row>
     <row r="83" spans="3:3">
-      <c r="C83" s="2"/>
+      <c r="C83" s="2">
+        <f t="shared" si="0"/>
+        <v>41156</v>
+      </c>
     </row>
     <row r="84" spans="3:3">
-      <c r="C84" s="2"/>
+      <c r="C84" s="2">
+        <f t="shared" si="0"/>
+        <v>41157</v>
+      </c>
     </row>
     <row r="85" spans="3:3">
-      <c r="C85" s="2"/>
+      <c r="C85" s="2">
+        <f t="shared" si="0"/>
+        <v>41158</v>
+      </c>
     </row>
     <row r="86" spans="3:3">
-      <c r="C86" s="2"/>
+      <c r="C86" s="2">
+        <f t="shared" si="0"/>
+        <v>41159</v>
+      </c>
     </row>
     <row r="87" spans="3:3">
-      <c r="C87" s="2"/>
+      <c r="C87" s="2">
+        <f t="shared" si="0"/>
+        <v>41160</v>
+      </c>
     </row>
     <row r="88" spans="3:3">
-      <c r="C88" s="2"/>
+      <c r="C88" s="2">
+        <f t="shared" si="0"/>
+        <v>41161</v>
+      </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" s="2"/>
@@ -1307,13 +1408,38 @@
     <row r="96" spans="3:3">
       <c r="C96" s="2"/>
     </row>
-    <row r="126" spans="3:3">
+    <row r="117" spans="3:5">
+      <c r="C117" s="2"/>
+      <c r="D117" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117">
+        <f>SUM(E5:E115)</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="118" spans="3:5">
+      <c r="C118" s="2"/>
+    </row>
+    <row r="119" spans="3:5">
+      <c r="C119" s="2"/>
+    </row>
+    <row r="120" spans="3:5">
+      <c r="C120" s="2"/>
+      <c r="D120" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="3:5">
       <c r="C126" s="2"/>
     </row>
-    <row r="127" spans="3:3">
+    <row r="127" spans="3:5">
       <c r="C127" s="2"/>
     </row>
-    <row r="128" spans="3:3">
+    <row r="128" spans="3:5">
       <c r="C128" s="2"/>
     </row>
     <row r="129" spans="3:3">

</xml_diff>

<commit_message>
Timesheet_entries from 1/09/2012 to 9/9/2012
</commit_message>
<xml_diff>
--- a/Time_sheet.xlsx
+++ b/Time_sheet.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="20">
   <si>
     <t>Date</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t xml:space="preserve">Report for  2nd deliverable </t>
+  </si>
+  <si>
+    <t>deciding the topic for case study</t>
+  </si>
+  <si>
+    <t>Work on the 1st BDW component</t>
   </si>
 </sst>
 </file>
@@ -423,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:E542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="E121" sqref="E121"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86:D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1335,77 +1341,131 @@
         <f t="shared" si="0"/>
         <v>41153</v>
       </c>
-    </row>
-    <row r="81" spans="3:3">
+      <c r="D80" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5">
       <c r="C81" s="2">
         <f t="shared" si="0"/>
         <v>41154</v>
       </c>
-    </row>
-    <row r="82" spans="3:3">
+      <c r="D81" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5">
       <c r="C82" s="2">
         <f t="shared" si="0"/>
         <v>41155</v>
       </c>
-    </row>
-    <row r="83" spans="3:3">
+      <c r="D82" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5">
       <c r="C83" s="2">
         <f t="shared" si="0"/>
         <v>41156</v>
       </c>
-    </row>
-    <row r="84" spans="3:3">
+      <c r="D83" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5">
       <c r="C84" s="2">
         <f t="shared" si="0"/>
         <v>41157</v>
       </c>
-    </row>
-    <row r="85" spans="3:3">
+      <c r="D84" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5">
       <c r="C85" s="2">
         <f t="shared" si="0"/>
         <v>41158</v>
       </c>
-    </row>
-    <row r="86" spans="3:3">
+      <c r="D85" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5">
       <c r="C86" s="2">
         <f t="shared" si="0"/>
         <v>41159</v>
       </c>
-    </row>
-    <row r="87" spans="3:3">
+      <c r="D86" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5">
       <c r="C87" s="2">
         <f t="shared" si="0"/>
         <v>41160</v>
       </c>
-    </row>
-    <row r="88" spans="3:3">
+      <c r="D87" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5">
       <c r="C88" s="2">
         <f t="shared" si="0"/>
         <v>41161</v>
       </c>
-    </row>
-    <row r="89" spans="3:3">
+      <c r="D88" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5">
       <c r="C89" s="2"/>
     </row>
-    <row r="90" spans="3:3">
+    <row r="90" spans="3:5">
       <c r="C90" s="2"/>
     </row>
-    <row r="91" spans="3:3">
+    <row r="91" spans="3:5">
       <c r="C91" s="2"/>
     </row>
-    <row r="92" spans="3:3">
+    <row r="92" spans="3:5">
       <c r="C92" s="2"/>
     </row>
-    <row r="93" spans="3:3">
+    <row r="93" spans="3:5">
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="3:3">
+    <row r="94" spans="3:5">
       <c r="C94" s="2"/>
     </row>
-    <row r="95" spans="3:3">
+    <row r="95" spans="3:5">
       <c r="C95" s="2"/>
     </row>
-    <row r="96" spans="3:3">
+    <row r="96" spans="3:5">
       <c r="C96" s="2"/>
     </row>
     <row r="117" spans="3:5">
@@ -1415,7 +1475,7 @@
       </c>
       <c r="E117">
         <f>SUM(E5:E115)</f>
-        <v>89</v>
+        <v>94</v>
       </c>
     </row>
     <row r="118" spans="3:5">
@@ -1430,7 +1490,7 @@
         <v>12</v>
       </c>
       <c r="E120">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
     <row r="126" spans="3:5">

</xml_diff>